<commit_message>
Update Payroll Data 11-16
Update Payroll Data 11-16
</commit_message>
<xml_diff>
--- a/Sales and Staffing Charts.xlsx
+++ b/Sales and Staffing Charts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://culinarystaffing-my.sharepoint.com/personal/jake_golivestaffing_com/Documents/Documents/GitHub/GoLive_Staffing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{AE5846BF-940B-4D2C-884D-E857B5928A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD6021C4-D549-42EA-BC75-0088D62D59BB}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{AE5846BF-940B-4D2C-884D-E857B5928A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A941962-4C39-46CA-ACB8-02ACB00BE11C}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{A3B2B6D9-7C24-445E-A372-57A39B7AE13F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A3B2B6D9-7C24-445E-A372-57A39B7AE13F}"/>
   </bookViews>
   <sheets>
     <sheet name="Revenue" sheetId="1" r:id="rId1"/>
@@ -502,9 +502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F816EB9-28A4-4EE2-B083-40DDC67AF2B4}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1437,16 +1435,16 @@
         <v>45977</v>
       </c>
       <c r="B47" s="6">
-        <v>444444.44</v>
+        <v>298612.32999999961</v>
       </c>
       <c r="C47" s="6">
         <v>358939.24000000005</v>
       </c>
       <c r="D47" s="6">
-        <v>44444.44</v>
+        <v>43047.63</v>
       </c>
       <c r="E47" s="7">
-        <v>0.44440000000000002</v>
+        <v>0.14419999999999999</v>
       </c>
       <c r="F47" s="7"/>
     </row>
@@ -1531,8 +1529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC1FE54-5241-4EDC-8539-E8BDF3481B66}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2471,7 +2469,7 @@
         <v>1241</v>
       </c>
       <c r="C47">
-        <v>1044</v>
+        <v>1174</v>
       </c>
       <c r="E47" s="3">
         <v>45977</v>
@@ -2480,7 +2478,7 @@
         <v>0.96879999999999999</v>
       </c>
       <c r="G47">
-        <v>0.44440000000000002</v>
+        <v>0.87290000000000001</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.75">

</xml_diff>